<commit_message>
updated data for 12/10/2021
</commit_message>
<xml_diff>
--- a/B8 Tables/AAMC Table B-8 Merged.xlsx
+++ b/B8 Tables/AAMC Table B-8 Merged.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TooFastDan\Documents\MD_PhD Application\Python Analysis\B8 Tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{348535AB-8E5C-4B88-B6BF-5ADE34BE8577}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D1E2258-0D11-4FEB-A116-03B54B8A3C5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="6075" windowWidth="29040" windowHeight="16440" firstSheet="6" activeTab="6" xr2:uid="{EFF248D5-F459-4937-B6C3-A6CF642F6133}"/>
+    <workbookView xWindow="-120" yWindow="480" windowWidth="38640" windowHeight="21240" activeTab="4" xr2:uid="{EFF248D5-F459-4937-B6C3-A6CF642F6133}"/>
   </bookViews>
   <sheets>
     <sheet name="2016-2017" sheetId="1" r:id="rId1"/>
@@ -21,10 +21,20 @@
     <sheet name="2021-2022" sheetId="6" r:id="rId6"/>
     <sheet name="Totals" sheetId="7" r:id="rId7"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'2020-2021'!$A$1:$L$156</definedName>
+  </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -1131,7 +1141,7 @@
   <dimension ref="A1:L146"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O15" sqref="O15"/>
+      <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18165,8 +18175,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C451A3C0-47E7-4178-842D-E80E5427F25E}">
   <dimension ref="A1:L154"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+    <sheetView topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="B54" sqref="B54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -24046,8 +24056,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0871BA58-714A-4A2F-954D-8475204EB58C}">
   <dimension ref="A1:L156"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:L1"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="R15" sqref="R15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -30070,7 +30080,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF5EC771-6F68-418D-84D4-6ED72D58CAD4}">
   <dimension ref="A1:M15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>

</xml_diff>